<commit_message>
- Add labs 2 + 3.
</commit_message>
<xml_diff>
--- a/Reports/tables.xlsx
+++ b/Reports/tables.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Winda_BB_2025\SSD_backup\Univer\Sharaga 15 Term\СУЧАСНІ КОНЦЕПЦІЇ СТВОРЕННЯ ІНТЕЛЕКТУАЛЬНИХ ІНФОРМАЦІЙНИХ СИСТЕМ\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Winda_BB_2025\SSD_backup\Univer\Sharaga 15 Term\MCCIIS\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A8E9D7-D7A1-44C2-A105-CC77D26E1986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A42717-4F2D-4892-BAC8-20AAE9C31277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35505" yWindow="2895" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34905" yWindow="2865" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lab1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lab2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="37">
   <si>
     <t>N = 20</t>
   </si>
@@ -115,6 +116,39 @@
   </si>
   <si>
     <t>Насичений</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Max age H</t>
+  </si>
+  <si>
+    <t>Max age P</t>
+  </si>
+  <si>
+    <t>1-1 N=10; P=0; NP=0; H=3; P=20; I=20</t>
+  </si>
+  <si>
+    <t>1-2 N=16; P=120; NP=3; H=1; P=0; I=20</t>
+  </si>
+  <si>
+    <t>2 N=64; P=1500; NP=0; H=120; P=120; I=60</t>
+  </si>
+  <si>
+    <t>Reprod P</t>
+  </si>
+  <si>
+    <t>Reprod H</t>
+  </si>
+  <si>
+    <t>3 N=64; P=2200; NP=1; H=180; P=45; I=100</t>
+  </si>
+  <si>
+    <t>4 N=64; P=2200; NP=0; H=200; P=400; I=60</t>
   </si>
 </sst>
 </file>
@@ -551,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -585,14 +619,95 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -600,86 +715,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -963,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,56 +1023,56 @@
       </c>
     </row>
     <row r="4" spans="2:24" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="13" t="s">
+      <c r="D4" s="40"/>
+      <c r="E4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="40"/>
+      <c r="G4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="15"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="13" t="s">
+      <c r="L4" s="40"/>
+      <c r="M4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="14"/>
-      <c r="O4" s="13" t="s">
+      <c r="N4" s="40"/>
+      <c r="O4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="15"/>
+      <c r="P4" s="38"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="16" t="s">
+      <c r="R4" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="18" t="s">
+      <c r="S4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="T4" s="14"/>
-      <c r="U4" s="13" t="s">
+      <c r="T4" s="40"/>
+      <c r="U4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="V4" s="14"/>
-      <c r="W4" s="13" t="s">
+      <c r="V4" s="40"/>
+      <c r="W4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="X4" s="15"/>
+      <c r="X4" s="38"/>
     </row>
     <row r="5" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1050,7 +1092,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="5"/>
-      <c r="J5" s="17"/>
+      <c r="J5" s="44"/>
       <c r="K5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1070,7 +1112,7 @@
         <v>3</v>
       </c>
       <c r="Q5" s="5"/>
-      <c r="R5" s="17"/>
+      <c r="R5" s="44"/>
       <c r="S5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1380,56 +1422,56 @@
       </c>
     </row>
     <row r="13" spans="2:24" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="40"/>
+      <c r="E13" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="13" t="s">
+      <c r="F13" s="40"/>
+      <c r="G13" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="15"/>
+      <c r="H13" s="38"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="16" t="s">
+      <c r="J13" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="13" t="s">
+      <c r="L13" s="40"/>
+      <c r="M13" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="N13" s="14"/>
-      <c r="O13" s="13" t="s">
+      <c r="N13" s="40"/>
+      <c r="O13" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="P13" s="15"/>
+      <c r="P13" s="38"/>
       <c r="Q13" s="5"/>
-      <c r="R13" s="16" t="s">
+      <c r="R13" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="S13" s="18" t="s">
+      <c r="S13" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="T13" s="14"/>
-      <c r="U13" s="13" t="s">
+      <c r="T13" s="40"/>
+      <c r="U13" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="V13" s="14"/>
-      <c r="W13" s="13" t="s">
+      <c r="V13" s="40"/>
+      <c r="W13" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="X13" s="15"/>
+      <c r="X13" s="38"/>
     </row>
     <row r="14" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="20"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="6" t="s">
         <v>2</v>
       </c>
@@ -1449,7 +1491,7 @@
         <v>3</v>
       </c>
       <c r="I14" s="5"/>
-      <c r="J14" s="17"/>
+      <c r="J14" s="44"/>
       <c r="K14" s="6" t="s">
         <v>2</v>
       </c>
@@ -1469,7 +1511,7 @@
         <v>3</v>
       </c>
       <c r="Q14" s="5"/>
-      <c r="R14" s="17"/>
+      <c r="R14" s="44"/>
       <c r="S14" s="6" t="s">
         <v>2</v>
       </c>
@@ -1769,448 +1811,456 @@
     </row>
     <row r="20" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="H21" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="25">
+      <c r="B22" s="17">
         <v>20</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="31">
+      <c r="E22" s="23">
         <v>10</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="23">
         <v>50</v>
       </c>
-      <c r="G22" s="31">
+      <c r="G22" s="23">
         <v>36.018500000000003</v>
       </c>
-      <c r="H22" s="32">
+      <c r="H22" s="24">
         <v>30</v>
       </c>
-      <c r="J22">
-        <f>(G22+G25)/2</f>
-        <v>36.642700000000005</v>
-      </c>
     </row>
     <row r="23" spans="2:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="26">
+      <c r="B23" s="18">
         <v>20</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="34">
+      <c r="E23" s="26">
         <v>10</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="26">
         <v>100</v>
       </c>
-      <c r="G23" s="34">
+      <c r="G23" s="26">
         <v>35.957700000000003</v>
       </c>
-      <c r="H23" s="35">
+      <c r="H23" s="27">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="27">
+      <c r="B24" s="19">
         <v>20</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="37">
+      <c r="E24" s="29">
         <v>100</v>
       </c>
-      <c r="F24" s="37">
+      <c r="F24" s="29">
         <v>200</v>
       </c>
-      <c r="G24" s="37">
+      <c r="G24" s="29">
         <v>35.7301</v>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="30">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="2:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="28">
+      <c r="B25" s="20">
         <v>20</v>
       </c>
-      <c r="C25" s="39">
+      <c r="C25" s="31">
         <v>10</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="40">
+      <c r="E25" s="32">
         <v>10</v>
       </c>
-      <c r="F25" s="40">
+      <c r="F25" s="32">
         <v>50</v>
       </c>
-      <c r="G25" s="40">
+      <c r="G25" s="32">
         <v>37.2669</v>
       </c>
-      <c r="H25" s="41">
+      <c r="H25" s="33">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="26">
+      <c r="B26" s="18">
         <v>20</v>
       </c>
-      <c r="C26" s="33">
+      <c r="C26" s="25">
         <v>10</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="34">
+      <c r="E26" s="26">
         <v>10</v>
       </c>
-      <c r="F26" s="34">
+      <c r="F26" s="26">
         <v>100</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G26" s="26">
         <v>36.820300000000003</v>
       </c>
-      <c r="H26" s="35">
+      <c r="H26" s="27">
         <v>55</v>
       </c>
     </row>
     <row r="27" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="29">
+      <c r="B27" s="21">
         <v>20</v>
       </c>
-      <c r="C27" s="42">
+      <c r="C27" s="34">
         <v>10</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D27" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="43">
+      <c r="E27" s="35">
         <v>100</v>
       </c>
-      <c r="F27" s="43">
+      <c r="F27" s="35">
         <v>200</v>
       </c>
-      <c r="G27" s="43">
+      <c r="G27" s="35">
         <v>35.7301</v>
       </c>
-      <c r="H27" s="44">
+      <c r="H27" s="36">
         <v>63</v>
       </c>
     </row>
     <row r="28" spans="2:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="25">
+      <c r="B28" s="17">
         <v>50</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="31">
+      <c r="E28" s="23">
         <v>10</v>
       </c>
-      <c r="F28" s="31">
+      <c r="F28" s="23">
         <v>50</v>
       </c>
-      <c r="G28" s="31">
+      <c r="G28" s="23">
         <v>56.783200000000001</v>
       </c>
-      <c r="H28" s="32">
+      <c r="H28" s="24">
         <v>42</v>
       </c>
     </row>
     <row r="29" spans="2:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="26">
+      <c r="B29" s="18">
         <v>50</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="26">
         <v>25</v>
       </c>
-      <c r="F29" s="34">
+      <c r="F29" s="26">
         <v>100</v>
       </c>
-      <c r="G29" s="34">
+      <c r="G29" s="26">
         <v>55.911799999999999</v>
       </c>
-      <c r="H29" s="35">
+      <c r="H29" s="27">
         <v>65</v>
       </c>
     </row>
     <row r="30" spans="2:24" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="27">
+      <c r="B30" s="19">
         <v>50</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="37">
+      <c r="E30" s="29">
         <v>100</v>
       </c>
-      <c r="F30" s="37">
+      <c r="F30" s="29">
         <v>200</v>
       </c>
-      <c r="G30" s="37">
+      <c r="G30" s="29">
         <v>55.447499999999998</v>
       </c>
-      <c r="H30" s="38">
+      <c r="H30" s="30">
         <v>109</v>
       </c>
     </row>
     <row r="31" spans="2:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="28">
+      <c r="B31" s="20">
         <v>50</v>
       </c>
-      <c r="C31" s="39">
+      <c r="C31" s="31">
         <v>25</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="40">
+      <c r="E31" s="32">
         <v>10</v>
       </c>
-      <c r="F31" s="40">
+      <c r="F31" s="32">
         <v>50</v>
       </c>
-      <c r="G31" s="40">
+      <c r="G31" s="32">
         <v>59.401699999999998</v>
       </c>
-      <c r="H31" s="41">
+      <c r="H31" s="33">
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="2:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="26">
+      <c r="B32" s="18">
         <v>50</v>
       </c>
-      <c r="C32" s="33">
+      <c r="C32" s="25">
         <v>25</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="26">
         <v>25</v>
       </c>
-      <c r="F32" s="34">
+      <c r="F32" s="26">
         <v>100</v>
       </c>
-      <c r="G32" s="34">
+      <c r="G32" s="26">
         <v>56.541800000000002</v>
       </c>
-      <c r="H32" s="35">
+      <c r="H32" s="27">
         <v>36</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="29">
+      <c r="B33" s="21">
         <v>50</v>
       </c>
-      <c r="C33" s="42">
+      <c r="C33" s="34">
         <v>25</v>
       </c>
-      <c r="D33" s="43" t="s">
+      <c r="D33" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="35">
         <v>100</v>
       </c>
-      <c r="F33" s="43">
+      <c r="F33" s="35">
         <v>200</v>
       </c>
-      <c r="G33" s="43">
+      <c r="G33" s="35">
         <v>56.322200000000002</v>
       </c>
-      <c r="H33" s="44">
+      <c r="H33" s="36">
         <v>82</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" s="25">
+      <c r="B34" s="17">
         <v>100</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="31" t="s">
+      <c r="D34" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="23">
         <v>10</v>
       </c>
-      <c r="F34" s="31">
+      <c r="F34" s="23">
         <v>50</v>
       </c>
-      <c r="G34" s="31">
+      <c r="G34" s="23">
         <v>87.653199999999998</v>
       </c>
-      <c r="H34" s="32">
+      <c r="H34" s="24">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B35" s="26">
+      <c r="B35" s="18">
         <v>100</v>
       </c>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="26">
         <v>50</v>
       </c>
-      <c r="F35" s="34">
+      <c r="F35" s="26">
         <v>100</v>
       </c>
-      <c r="G35" s="34">
+      <c r="G35" s="26">
         <v>87.363299999999995</v>
       </c>
-      <c r="H35" s="35">
+      <c r="H35" s="27">
         <v>73</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="27">
+      <c r="B36" s="19">
         <v>100</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="37" t="s">
+      <c r="D36" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E36" s="37">
+      <c r="E36" s="29">
         <v>100</v>
       </c>
-      <c r="F36" s="37">
+      <c r="F36" s="29">
         <v>200</v>
       </c>
-      <c r="G36" s="37">
+      <c r="G36" s="29">
         <v>84.848799999999997</v>
       </c>
-      <c r="H36" s="38">
+      <c r="H36" s="30">
         <v>122</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B37" s="25">
+      <c r="B37" s="17">
         <v>100</v>
       </c>
-      <c r="C37" s="30">
+      <c r="C37" s="22">
         <v>50</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="31">
+      <c r="E37" s="23">
         <v>10</v>
       </c>
-      <c r="F37" s="31">
+      <c r="F37" s="23">
         <v>50</v>
       </c>
-      <c r="G37" s="31">
+      <c r="G37" s="23">
         <v>91.223699999999994</v>
       </c>
-      <c r="H37" s="32">
+      <c r="H37" s="24">
         <v>43</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="26">
+      <c r="B38" s="18">
         <v>100</v>
       </c>
-      <c r="C38" s="33">
+      <c r="C38" s="25">
         <v>50</v>
       </c>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="34">
+      <c r="E38" s="26">
         <v>50</v>
       </c>
-      <c r="F38" s="34">
+      <c r="F38" s="26">
         <v>100</v>
       </c>
-      <c r="G38" s="34">
+      <c r="G38" s="26">
         <v>88.061199999999999</v>
       </c>
-      <c r="H38" s="35">
+      <c r="H38" s="27">
         <v>52</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="27">
+      <c r="B39" s="19">
         <v>100</v>
       </c>
-      <c r="C39" s="36">
+      <c r="C39" s="28">
         <v>50</v>
       </c>
-      <c r="D39" s="37" t="s">
+      <c r="D39" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E39" s="37">
+      <c r="E39" s="29">
         <v>100</v>
       </c>
-      <c r="F39" s="37">
+      <c r="F39" s="29">
         <v>200</v>
       </c>
-      <c r="G39" s="37">
+      <c r="G39" s="29">
         <v>86.990200000000002</v>
       </c>
-      <c r="H39" s="38">
+      <c r="H39" s="30">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:V13"/>
     <mergeCell ref="W4:X4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
@@ -2223,20 +2273,786 @@
     <mergeCell ref="R4:R5"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="U13:V13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F563422C-E459-42F8-9ECB-2819CD898AA3}">
+  <dimension ref="B3:N37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>20</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3</v>
+      </c>
+      <c r="F5" s="9">
+        <v>20</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="8">
+        <v>6</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9">
+        <v>20</v>
+      </c>
+      <c r="N5" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2</v>
+      </c>
+      <c r="K6" s="10">
+        <v>9</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>20</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>20</v>
+      </c>
+      <c r="J7" s="2">
+        <v>3</v>
+      </c>
+      <c r="K7" s="10">
+        <v>8</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>20</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>20</v>
+      </c>
+      <c r="J8" s="3">
+        <v>4</v>
+      </c>
+      <c r="K8" s="10">
+        <v>8</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>20</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>20</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>20</v>
+      </c>
+      <c r="J9" s="2">
+        <v>5</v>
+      </c>
+      <c r="K9" s="10">
+        <v>5</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>20</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="48">
+        <f>AVERAGE(C5:C9)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="48">
+        <f>AVERAGE(D5:D9)</f>
+        <v>20</v>
+      </c>
+      <c r="E10" s="48">
+        <f t="shared" ref="C10:F10" si="0">AVERAGE(E5:E9)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F10" s="48">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="48">
+        <f>AVERAGE(K5:K9)</f>
+        <v>7.2</v>
+      </c>
+      <c r="L10" s="48">
+        <f t="shared" ref="L10:N10" si="1">AVERAGE(L5:L9)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="48">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="N10" s="48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>6</v>
+      </c>
+      <c r="D14" s="9">
+        <v>58</v>
+      </c>
+      <c r="E14" s="9">
+        <v>60</v>
+      </c>
+      <c r="F14" s="9">
+        <v>60</v>
+      </c>
+      <c r="G14" s="9">
+        <v>84</v>
+      </c>
+      <c r="H14" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="10">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1">
+        <v>63</v>
+      </c>
+      <c r="E15" s="1">
+        <v>60</v>
+      </c>
+      <c r="F15" s="1">
+        <v>60</v>
+      </c>
+      <c r="G15" s="1">
+        <v>94</v>
+      </c>
+      <c r="H15" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="10">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>58</v>
+      </c>
+      <c r="E16" s="1">
+        <v>60</v>
+      </c>
+      <c r="F16" s="1">
+        <v>60</v>
+      </c>
+      <c r="G16" s="1">
+        <v>90</v>
+      </c>
+      <c r="H16" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>4</v>
+      </c>
+      <c r="C17" s="10">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>62</v>
+      </c>
+      <c r="E17" s="1">
+        <v>60</v>
+      </c>
+      <c r="F17" s="1">
+        <v>60</v>
+      </c>
+      <c r="G17" s="1">
+        <v>94</v>
+      </c>
+      <c r="H17" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>67</v>
+      </c>
+      <c r="E18" s="1">
+        <v>60</v>
+      </c>
+      <c r="F18" s="1">
+        <v>60</v>
+      </c>
+      <c r="G18" s="1">
+        <v>99</v>
+      </c>
+      <c r="H18" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="48">
+        <f>AVERAGE(C14:C18)</f>
+        <v>5</v>
+      </c>
+      <c r="D19" s="48">
+        <f t="shared" ref="D19:H19" si="2">AVERAGE(D14:D18)</f>
+        <v>61.6</v>
+      </c>
+      <c r="E19" s="48">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="F19" s="48">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="G19" s="48">
+        <f t="shared" si="2"/>
+        <v>92.2</v>
+      </c>
+      <c r="H19" s="48">
+        <f t="shared" si="2"/>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
+        <v>752</v>
+      </c>
+      <c r="E23" s="9">
+        <v>74</v>
+      </c>
+      <c r="F23" s="9">
+        <v>100</v>
+      </c>
+      <c r="G23" s="9">
+        <v>3893</v>
+      </c>
+      <c r="H23" s="9">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="3">
+        <v>2</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>863</v>
+      </c>
+      <c r="E24" s="1">
+        <v>67</v>
+      </c>
+      <c r="F24" s="1">
+        <v>100</v>
+      </c>
+      <c r="G24" s="1">
+        <v>4272</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="2">
+        <v>3</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>788</v>
+      </c>
+      <c r="E25" s="1">
+        <v>81</v>
+      </c>
+      <c r="F25" s="1">
+        <v>100</v>
+      </c>
+      <c r="G25" s="1">
+        <v>4079</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="3">
+        <v>4</v>
+      </c>
+      <c r="C26" s="10">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>774</v>
+      </c>
+      <c r="E26" s="1">
+        <v>70</v>
+      </c>
+      <c r="F26" s="1">
+        <v>100</v>
+      </c>
+      <c r="G26" s="1">
+        <v>4008</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <v>5</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>800</v>
+      </c>
+      <c r="E27" s="1">
+        <v>71</v>
+      </c>
+      <c r="F27" s="1">
+        <v>100</v>
+      </c>
+      <c r="G27" s="1">
+        <v>4112</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="48">
+        <f>AVERAGE(C23:C27)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="48">
+        <f t="shared" ref="D28:H28" si="3">AVERAGE(D23:D27)</f>
+        <v>795.4</v>
+      </c>
+      <c r="E28" s="48">
+        <f t="shared" si="3"/>
+        <v>72.599999999999994</v>
+      </c>
+      <c r="F28" s="48">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="G28" s="48">
+        <f t="shared" si="3"/>
+        <v>4072.8</v>
+      </c>
+      <c r="H28" s="48">
+        <f t="shared" si="3"/>
+        <v>1060.8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="8">
+        <v>0</v>
+      </c>
+      <c r="D32" s="9">
+        <v>64</v>
+      </c>
+      <c r="E32" s="9">
+        <v>22</v>
+      </c>
+      <c r="F32" s="9">
+        <v>60</v>
+      </c>
+      <c r="G32" s="9">
+        <v>106</v>
+      </c>
+      <c r="H32" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="3">
+        <v>2</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>76</v>
+      </c>
+      <c r="E33" s="1">
+        <v>22</v>
+      </c>
+      <c r="F33" s="1">
+        <v>60</v>
+      </c>
+      <c r="G33" s="1">
+        <v>115</v>
+      </c>
+      <c r="H33" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="2">
+        <v>3</v>
+      </c>
+      <c r="C34" s="10">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>69</v>
+      </c>
+      <c r="E34" s="1">
+        <v>31</v>
+      </c>
+      <c r="F34" s="1">
+        <v>60</v>
+      </c>
+      <c r="G34" s="1">
+        <v>106</v>
+      </c>
+      <c r="H34" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="3">
+        <v>4</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <v>54</v>
+      </c>
+      <c r="E35" s="1">
+        <v>24</v>
+      </c>
+      <c r="F35" s="1">
+        <v>60</v>
+      </c>
+      <c r="G35" s="1">
+        <v>103</v>
+      </c>
+      <c r="H35" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="2">
+        <v>5</v>
+      </c>
+      <c r="C36" s="10">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>58</v>
+      </c>
+      <c r="E36" s="1">
+        <v>22</v>
+      </c>
+      <c r="F36" s="1">
+        <v>60</v>
+      </c>
+      <c r="G36" s="1">
+        <v>112</v>
+      </c>
+      <c r="H36" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="48">
+        <f>AVERAGE(C32:C36)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="48">
+        <f t="shared" ref="D37:H37" si="4">AVERAGE(D32:D36)</f>
+        <v>64.2</v>
+      </c>
+      <c r="E37" s="48">
+        <f t="shared" si="4"/>
+        <v>24.2</v>
+      </c>
+      <c r="F37" s="48">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="G37" s="48">
+        <f t="shared" si="4"/>
+        <v>108.4</v>
+      </c>
+      <c r="H37" s="48">
+        <f t="shared" si="4"/>
+        <v>13.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>